<commit_message>
Fix some bug and add report feature
</commit_message>
<xml_diff>
--- a/DetailDesignByPOS.xlsx
+++ b/DetailDesignByPOS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MotelManagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\RMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Room Booking" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="58">
   <si>
     <t>Project Name</t>
   </si>
@@ -209,6 +209,33 @@
   <si>
     <t>นายประหยัด</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Room name</t>
+  </si>
+  <si>
+    <t>Booking type</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Temporaly</t>
+  </si>
+  <si>
+    <t>5/23/2014:20.00 to 5/23/2014:22.00</t>
+  </si>
+  <si>
+    <t>Total income</t>
+  </si>
+  <si>
+    <t>Booked by</t>
+  </si>
+  <si>
+    <t>padungsak suntonphon</t>
+  </si>
 </sst>
 </file>
 
@@ -381,7 +408,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -416,14 +443,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6887,44 +6916,6 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>389398</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>104352</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="200025" y="2886075"/>
-          <a:ext cx="9019048" cy="3380952"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -7677,7 +7668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -9173,10 +9164,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="24"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="20"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -9584,7 +9575,7 @@
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="25">
         <v>41772</v>
       </c>
     </row>
@@ -9675,10 +9666,10 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="24"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="20"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -9838,7 +9829,7 @@
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="25">
         <v>41772</v>
       </c>
     </row>
@@ -10128,16 +10119,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.875" style="1" customWidth="1"/>
     <col min="3" max="3" width="38.75" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.75" style="1" customWidth="1"/>
     <col min="5" max="5" width="20.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="22" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
@@ -10169,8 +10160,8 @@
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="25">
-        <v>41772</v>
+      <c r="B4" s="24">
+        <v>41782</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -10275,27 +10266,57 @@
       <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="A18" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>56</v>
+      </c>
       <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
+      <c r="A19" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="22">
+        <v>300</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>57</v>
+      </c>
       <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
+      <c r="A20" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="22">
+        <v>300</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>57</v>
+      </c>
       <c r="F20" s="13"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -10308,8 +10329,12 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
+      <c r="B22" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="10">
+        <v>600</v>
+      </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="13"/>

</xml_diff>